<commit_message>
updated case and bom
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\work-sign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B16DF8-631C-48E6-BEBA-D2F53D2824E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2320B62D-03B2-430D-A111-68176F63295C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{65FF75E3-ED98-4EE0-A10A-1D060FB74263}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Item</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>12v 2A Power Supply</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005005321856209.html</t>
+  </si>
+  <si>
+    <t>5M Silver Plated Copper Wire 24AWG</t>
+  </si>
+  <si>
+    <t>for connecting esp32 and led strips</t>
   </si>
 </sst>
 </file>
@@ -962,16 +971,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD5727A-81B0-4FD1-B53A-EDF9F932D237}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="48.21875" customWidth="1"/>
@@ -1101,12 +1110,38 @@
         <v>28.75</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3.46</v>
+      </c>
+      <c r="E6">
+        <f>C6*D6</f>
+        <v>3.46</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <f>ROUND(E6*1.12,2)+G5</f>
+        <v>32.630000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{8D4DE6EF-DBE7-4E2E-8DD7-E4A5DF6306FE}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{BAC3F642-A000-4A21-847E-25A06488169A}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{E1729C5F-3319-4B4C-AD5A-4218366D0EBD}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{E76D08EC-F8C5-41DC-8AD5-C2C1B1CA6E5F}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{8692D94E-AF95-4422-B8EE-D9118A6882CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>